<commit_message>
update results and outcomes excel to include only those who answered ACASI
</commit_message>
<xml_diff>
--- a/results/NHANES.xlsx
+++ b/results/NHANES.xlsx
@@ -38669,13 +38669,13 @@
         <v>1</v>
       </c>
       <c r="B4" s="35">
-        <v>0.011339480814351308</v>
+        <v>0.011339480814351309</v>
       </c>
       <c r="C4" s="36">
         <v>0.005669121431727665</v>
       </c>
       <c r="D4" s="37">
-        <v>0.0044639960048222455</v>
+        <v>0.0044639960048222446</v>
       </c>
       <c r="E4" s="38">
         <v>0.0036623157391362693</v>
@@ -38684,13 +38684,13 @@
         <v>0.0058565875853570752</v>
       </c>
       <c r="G4" s="40">
-        <v>0.011339480814351308</v>
+        <v>0.011339480814351309</v>
       </c>
       <c r="H4" s="41">
         <v>0.005669121431727665</v>
       </c>
       <c r="I4" s="42">
-        <v>0.0044639960048222455</v>
+        <v>0.0044639960048222446</v>
       </c>
       <c r="J4" s="43">
         <v>0.0036623157391362693</v>
@@ -38704,13 +38704,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="46">
-        <v>9.8945309056738182</v>
+        <v>9.8945309056738164</v>
       </c>
       <c r="C5" s="47">
         <v>6.0418842240990465</v>
       </c>
       <c r="D5" s="48">
-        <v>5.2055555556964528</v>
+        <v>5.2055555556964537</v>
       </c>
       <c r="E5" s="49">
         <v>6.6956774734135562</v>
@@ -38719,13 +38719,13 @@
         <v>4.9237759565865735</v>
       </c>
       <c r="G5" s="51">
-        <v>78.292928147512697</v>
+        <v>78.292928147512683</v>
       </c>
       <c r="H5" s="52">
         <v>170.35229114202113</v>
       </c>
       <c r="I5" s="53">
-        <v>218.80898184974632</v>
+        <v>218.80898184974635</v>
       </c>
       <c r="J5" s="54">
         <v>266.35560243503113</v>
@@ -38739,7 +38739,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="57">
-        <v>2.936702105127576e-11</v>
+        <v>2.9367021051275863e-11</v>
       </c>
       <c r="C6" s="58">
         <v>9.6156295046234139e-07</v>
@@ -39055,10 +39055,10 @@
         <v>1</v>
       </c>
       <c r="B18" s="156">
-        <v>0.012084196739081267</v>
+        <v>0.012084196739081269</v>
       </c>
       <c r="C18" s="157">
-        <v>0.0097254705396680411</v>
+        <v>0.0097254705396680394</v>
       </c>
       <c r="D18" s="158">
         <v>0.009619783310862379</v>
@@ -39070,10 +39070,10 @@
         <v>0.012658646787858337</v>
       </c>
       <c r="G18" s="161">
-        <v>0.012084196739081267</v>
+        <v>0.012084196739081269</v>
       </c>
       <c r="H18" s="162">
-        <v>0.0097254705396680411</v>
+        <v>0.0097254705396680394</v>
       </c>
       <c r="I18" s="163">
         <v>0.009619783310862379</v>
@@ -39090,10 +39090,10 @@
         <v>2</v>
       </c>
       <c r="B19" s="167">
-        <v>15.397664284689748</v>
+        <v>15.397664284689746</v>
       </c>
       <c r="C19" s="168">
-        <v>11.909866900369162</v>
+        <v>11.909866900369163</v>
       </c>
       <c r="D19" s="169">
         <v>11.19751800594541</v>
@@ -39105,10 +39105,10 @@
         <v>17.869404356918377</v>
       </c>
       <c r="G19" s="172">
-        <v>67.355043370749144</v>
+        <v>67.355043370749129</v>
       </c>
       <c r="H19" s="173">
-        <v>90.912921562278626</v>
+        <v>90.91292156227864</v>
       </c>
       <c r="I19" s="174">
         <v>92.754927458270927</v>
@@ -39143,7 +39143,7 @@
         <v>4.71111259201947e-36</v>
       </c>
       <c r="H20" s="184">
-        <v>3.3596276809177587e-40</v>
+        <v>3.3596276809177579e-40</v>
       </c>
       <c r="I20" s="185">
         <v>1.7723523190243331e-40</v>
@@ -39175,7 +39175,7 @@
         <v>0.20146033050316994</v>
       </c>
       <c r="G21" s="194">
-        <v>0.78805344332650273</v>
+        <v>0.78805344332650262</v>
       </c>
       <c r="H21" s="195">
         <v>0.86284229653167044</v>
@@ -39447,7 +39447,7 @@
         <v>0.0079218885590127477</v>
       </c>
       <c r="D33" s="279">
-        <v>0.0097172656464519554</v>
+        <v>0.0097172656464519537</v>
       </c>
       <c r="E33" s="280">
         <v>0.011230544222933668</v>
@@ -39462,7 +39462,7 @@
         <v>0.0079218885590127477</v>
       </c>
       <c r="I33" s="284">
-        <v>0.0097172656464519554</v>
+        <v>0.0097172656464519537</v>
       </c>
       <c r="J33" s="285">
         <v>0.011230544222933668</v>
@@ -39482,7 +39482,7 @@
         <v>115.51084389446477</v>
       </c>
       <c r="D34" s="290">
-        <v>96.365038566006163</v>
+        <v>96.365038566006177</v>
       </c>
       <c r="E34" s="291">
         <v>82.530870569005955</v>
@@ -39497,7 +39497,7 @@
         <v>10.721681664393035</v>
       </c>
       <c r="I34" s="295">
-        <v>6.5445695875105558</v>
+        <v>6.5445695875105567</v>
       </c>
       <c r="J34" s="296">
         <v>6.5120092905399591</v>
@@ -39532,7 +39532,7 @@
         <v>4.0113122785471071e-12</v>
       </c>
       <c r="I35" s="306">
-        <v>2.2651483981536314e-07</v>
+        <v>2.2651483981536234e-07</v>
       </c>
       <c r="J35" s="307">
         <v>2.486151442472212e-07</v>
@@ -40228,10 +40228,10 @@
         <v>0.0050608179590481946</v>
       </c>
       <c r="D4" s="521">
-        <v>0.0062110865516259812</v>
+        <v>0.0062110865516259803</v>
       </c>
       <c r="E4" s="522">
-        <v>0.010684304766823593</v>
+        <v>0.010684304766823595</v>
       </c>
       <c r="F4" s="523">
         <v>0.009218935778462934</v>
@@ -40243,10 +40243,10 @@
         <v>0.0050608179590481946</v>
       </c>
       <c r="I4" s="526">
-        <v>0.0062110865516259812</v>
+        <v>0.0062110865516259803</v>
       </c>
       <c r="J4" s="527">
-        <v>0.010684304766823593</v>
+        <v>0.010684304766823595</v>
       </c>
       <c r="K4" s="528">
         <v>0.009218935778462934</v>
@@ -40266,7 +40266,7 @@
         <v>10.19101500543549</v>
       </c>
       <c r="E5" s="533">
-        <v>11.887242068990373</v>
+        <v>11.887242068990371</v>
       </c>
       <c r="F5" s="534">
         <v>3.1022544203207776</v>
@@ -40278,10 +40278,10 @@
         <v>189.64382166167951</v>
       </c>
       <c r="I5" s="537">
-        <v>150.81141052640854</v>
+        <v>150.81141052640857</v>
       </c>
       <c r="J5" s="538">
-        <v>81.707991483795738</v>
+        <v>81.707991483795723</v>
       </c>
       <c r="K5" s="539">
         <v>105.37013588921766</v>
@@ -40301,7 +40301,7 @@
         <v>1.4240937236449755e-11</v>
       </c>
       <c r="E6" s="544">
-        <v>2.8106785554067698e-13</v>
+        <v>2.81067855540679e-13</v>
       </c>
       <c r="F6" s="545">
         <v>0.0039939838206538621</v>
@@ -40316,7 +40316,7 @@
         <v>3.2284609629470947e-47</v>
       </c>
       <c r="J6" s="549">
-        <v>1.0084577744525243e-38</v>
+        <v>1.0084577744525387e-38</v>
       </c>
       <c r="K6" s="550">
         <v>3.0338972016796548e-42</v>
@@ -40351,7 +40351,7 @@
         <v>0.92280916755632447</v>
       </c>
       <c r="J7" s="560">
-        <v>0.84959167359042131</v>
+        <v>0.8495916735904212</v>
       </c>
       <c r="K7" s="561">
         <v>0.9452887552405399</v>
@@ -40371,7 +40371,7 @@
         <v>0.077190832443675472</v>
       </c>
       <c r="E8" s="566">
-        <v>0.15040832640957882</v>
+        <v>0.15040832640957885</v>
       </c>
       <c r="F8" s="567">
         <v>0.054711244759460147</v>
@@ -40608,7 +40608,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="640">
-        <v>0.0079492342379016354</v>
+        <v>0.0079492342379016336</v>
       </c>
       <c r="C18" s="641">
         <v>0.016860227847952942</v>
@@ -40623,7 +40623,7 @@
         <v>0.021648873934160567</v>
       </c>
       <c r="G18" s="645">
-        <v>0.0079492342379016354</v>
+        <v>0.0079492342379016336</v>
       </c>
       <c r="H18" s="646">
         <v>0.016860227847952942</v>
@@ -40643,7 +40643,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="651">
-        <v>11.154172119493866</v>
+        <v>11.154172119493868</v>
       </c>
       <c r="C19" s="652">
         <v>13.399475776608229</v>
@@ -40658,7 +40658,7 @@
         <v>5.262416205812209</v>
       </c>
       <c r="G19" s="656">
-        <v>114.6441085792984</v>
+        <v>114.64410857929843</v>
       </c>
       <c r="H19" s="657">
         <v>45.911703705548852</v>
@@ -40678,7 +40678,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="662">
-        <v>1.4667859039252841e-12</v>
+        <v>1.4667859039252738e-12</v>
       </c>
       <c r="C20" s="663">
         <v>1.1356959753591775e-14</v>
@@ -40693,7 +40693,7 @@
         <v>9.2605592253502902e-06</v>
       </c>
       <c r="G20" s="667">
-        <v>2.0545469043796434e-43</v>
+        <v>2.0545469043796143e-43</v>
       </c>
       <c r="H20" s="668">
         <v>8.8146475538252595e-31</v>
@@ -40713,7 +40713,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="673">
-        <v>0.073754129258518666</v>
+        <v>0.073754129258518694</v>
       </c>
       <c r="C21" s="674">
         <v>0.19342817436963047</v>
@@ -40748,7 +40748,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="684">
-        <v>0.10624961973444048</v>
+        <v>0.10624961973444043</v>
       </c>
       <c r="C22" s="685">
         <v>0.2620922522631155</v>
@@ -40994,31 +40994,31 @@
         <v>1</v>
       </c>
       <c r="B33" s="761">
-        <v>0.0075293759577472665</v>
+        <v>0.0075293759577472648</v>
       </c>
       <c r="C33" s="762">
-        <v>0.0073645481251248318</v>
+        <v>0.00736454812512483</v>
       </c>
       <c r="D33" s="763">
         <v>0.0055596785140392497</v>
       </c>
       <c r="E33" s="764">
-        <v>0.0068181835626437938</v>
+        <v>0.0068181835626437946</v>
       </c>
       <c r="F33" s="765">
         <v>0.019127069099159032</v>
       </c>
       <c r="G33" s="766">
-        <v>0.0075293759577472665</v>
+        <v>0.0075293759577472648</v>
       </c>
       <c r="H33" s="767">
-        <v>0.0073645481251248318</v>
+        <v>0.00736454812512483</v>
       </c>
       <c r="I33" s="768">
         <v>0.0055596785140392497</v>
       </c>
       <c r="J33" s="769">
-        <v>0.0068181835626437938</v>
+        <v>0.0068181835626437946</v>
       </c>
       <c r="K33" s="770">
         <v>0.019127069099159032</v>
@@ -41029,10 +41029,10 @@
         <v>2</v>
       </c>
       <c r="B34" s="772">
-        <v>121.15200486565037</v>
+        <v>121.1520048656504</v>
       </c>
       <c r="C34" s="773">
-        <v>121.83993440804572</v>
+        <v>121.83993440804575</v>
       </c>
       <c r="D34" s="774">
         <v>170.95744135866008</v>
@@ -41044,16 +41044,16 @@
         <v>47.200243274738312</v>
       </c>
       <c r="G34" s="777">
-        <v>11.66112674203103</v>
+        <v>11.661126742031032</v>
       </c>
       <c r="H34" s="778">
-        <v>13.945721820937049</v>
+        <v>13.945721820937052</v>
       </c>
       <c r="I34" s="779">
         <v>8.9090738498738258</v>
       </c>
       <c r="J34" s="780">
-        <v>5.0796978392584515</v>
+        <v>5.0796978392584506</v>
       </c>
       <c r="K34" s="781">
         <v>5.0816821376589001</v>
@@ -41064,7 +41064,7 @@
         <v>3</v>
       </c>
       <c r="B35" s="783">
-        <v>3.5245624389882206e-44</v>
+        <v>3.5245624389881704e-44</v>
       </c>
       <c r="C35" s="784">
         <v>2.9415808244560199e-44</v>
@@ -41079,16 +41079,16 @@
         <v>3.6810540742235636e-31</v>
       </c>
       <c r="G35" s="788">
-        <v>4.6462804336533728e-13</v>
+        <v>4.6462804336533556e-13</v>
       </c>
       <c r="H35" s="789">
-        <v>3.7913709308373062e-15</v>
+        <v>3.7913709308372794e-15</v>
       </c>
       <c r="I35" s="790">
         <v>3.5360766673006642e-10</v>
       </c>
       <c r="J35" s="791">
-        <v>1.5761420186895024e-05</v>
+        <v>1.5761420186895081e-05</v>
       </c>
       <c r="K35" s="792">
         <v>1.5670709565319137e-05</v>
@@ -41380,34 +41380,34 @@
         <v>1</v>
       </c>
       <c r="B48" s="882">
-        <v>0.013361553547434211</v>
+        <v>0.013361553547434213</v>
       </c>
       <c r="C48" s="883">
         <v>0.01660025437379983</v>
       </c>
       <c r="D48" s="884">
-        <v>0.013930306724214464</v>
+        <v>0.013930306724214463</v>
       </c>
       <c r="E48" s="885">
         <v>0.013011252034562147</v>
       </c>
       <c r="F48" s="886">
-        <v>0.038165571914216288</v>
+        <v>0.038165571914216295</v>
       </c>
       <c r="G48" s="887">
-        <v>0.013361553547434211</v>
+        <v>0.013361553547434213</v>
       </c>
       <c r="H48" s="888">
         <v>0.01660025437379983</v>
       </c>
       <c r="I48" s="889">
-        <v>0.013930306724214464</v>
+        <v>0.013930306724214463</v>
       </c>
       <c r="J48" s="890">
         <v>0.013011252034562147</v>
       </c>
       <c r="K48" s="891">
-        <v>0.038165571914216288</v>
+        <v>0.038165571914216295</v>
       </c>
     </row>
     <row r="49">
@@ -41415,19 +41415,19 @@
         <v>2</v>
       </c>
       <c r="B49" s="893">
-        <v>41.573255897079527</v>
+        <v>41.57325589707952</v>
       </c>
       <c r="C49" s="894">
         <v>38.367388755464063</v>
       </c>
       <c r="D49" s="895">
-        <v>40.96891651369566</v>
+        <v>40.968916513695667</v>
       </c>
       <c r="E49" s="896">
         <v>60.998071256951278</v>
       </c>
       <c r="F49" s="897">
-        <v>15.188603259512272</v>
+        <v>15.188603259512268</v>
       </c>
       <c r="G49" s="898">
         <v>33.268340662029253</v>
@@ -41436,13 +41436,13 @@
         <v>21.872651998266754</v>
       </c>
       <c r="I49" s="900">
-        <v>30.817011807734779</v>
+        <v>30.817011807734783</v>
       </c>
       <c r="J49" s="901">
         <v>15.858483157925356</v>
       </c>
       <c r="K49" s="902">
-        <v>11.013021656463641</v>
+        <v>11.013021656463639</v>
       </c>
     </row>
     <row r="50">
@@ -41450,19 +41450,19 @@
         <v>3</v>
       </c>
       <c r="B50" s="904">
-        <v>2.0072075253211085e-29</v>
+        <v>2.0072075253211371e-29</v>
       </c>
       <c r="C50" s="905">
         <v>2.4919448299739273e-28</v>
       </c>
       <c r="D50" s="906">
-        <v>3.1802069122048138e-29</v>
+        <v>3.1802069122047914e-29</v>
       </c>
       <c r="E50" s="907">
         <v>1.0977432442661272e-34</v>
       </c>
       <c r="F50" s="908">
-        <v>3.4964745389397346e-16</v>
+        <v>3.4964745389397593e-16</v>
       </c>
       <c r="G50" s="909">
         <v>2.1435840914625068e-26</v>
@@ -41477,7 +41477,7 @@
         <v>1.0283217268725086e-16</v>
       </c>
       <c r="K50" s="913">
-        <v>2.0315982104209277e-12</v>
+        <v>2.0315982104209418e-12</v>
       </c>
     </row>
     <row r="51">
@@ -41532,7 +41532,7 @@
         <v>0.81890932308563069</v>
       </c>
       <c r="F52" s="930">
-        <v>0.65487396685224197</v>
+        <v>0.65487396685224208</v>
       </c>
       <c r="G52" s="931">
         <v>0.47187291703079276</v>
@@ -41547,7 +41547,7 @@
         <v>0.23410060436098409</v>
       </c>
       <c r="K52" s="935">
-        <v>0.49939978364665361</v>
+        <v>0.49939978364665366</v>
       </c>
     </row>
     <row r="53">
@@ -41742,7 +41742,7 @@
         <v>0.0067639678025120057</v>
       </c>
       <c r="C4" s="992">
-        <v>0.0049289688582017056</v>
+        <v>0.0049289688582017065</v>
       </c>
       <c r="D4" s="993">
         <v>0.0055704309799985748</v>
@@ -41751,7 +41751,7 @@
         <v>0.0067639678025120057</v>
       </c>
       <c r="F4" s="995">
-        <v>0.0049289688582017056</v>
+        <v>0.0049289688582017065</v>
       </c>
       <c r="G4" s="996">
         <v>0.0055704309799985748</v>
@@ -41765,7 +41765,7 @@
         <v>8.8219719670949797</v>
       </c>
       <c r="C5" s="999">
-        <v>7.9194667549810482</v>
+        <v>7.9194667549810465</v>
       </c>
       <c r="D5" s="1000">
         <v>7.8059987272194418</v>
@@ -41774,7 +41774,7 @@
         <v>139.02024567749811</v>
       </c>
       <c r="F5" s="1002">
-        <v>194.96272397666053</v>
+        <v>194.9627239766605</v>
       </c>
       <c r="G5" s="1003">
         <v>171.71332456942355</v>
@@ -41788,7 +41788,7 @@
         <v>4.4329477479932753e-10</v>
       </c>
       <c r="C6" s="1006">
-        <v>4.8828446069655125e-09</v>
+        <v>4.8828446069655472e-09</v>
       </c>
       <c r="D6" s="1007">
         <v>6.6494185415475938e-09</v>
@@ -41797,7 +41797,7 @@
         <v>4.3522817603187204e-46</v>
       </c>
       <c r="F6" s="1009">
-        <v>8.7952090496184133e-51</v>
+        <v>8.7952090496185379e-51</v>
       </c>
       <c r="G6" s="1010">
         <v>5.0971676705902015e-49</v>
@@ -41999,7 +41999,7 @@
         <v>0.0074609509860945429</v>
       </c>
       <c r="D18" s="1070">
-        <v>0.010596980441668805</v>
+        <v>0.010596980441668806</v>
       </c>
       <c r="E18" s="1071">
         <v>0.0084537259665295322</v>
@@ -42008,7 +42008,7 @@
         <v>0.0074609509860945429</v>
       </c>
       <c r="G18" s="1073">
-        <v>0.010596980441668805</v>
+        <v>0.010596980441668806</v>
       </c>
     </row>
     <row r="19">
@@ -42022,7 +42022,7 @@
         <v>16.199653638375203</v>
       </c>
       <c r="D19" s="1077">
-        <v>13.778849764766436</v>
+        <v>13.778849764766433</v>
       </c>
       <c r="E19" s="1078">
         <v>101.67589249106513</v>
@@ -42031,7 +42031,7 @@
         <v>117.83151770476385</v>
       </c>
       <c r="G19" s="1080">
-        <v>80.587654496000212</v>
+        <v>80.587654496000198</v>
       </c>
     </row>
     <row r="20">
@@ -42045,7 +42045,7 @@
         <v>5.5992250652195154e-17</v>
       </c>
       <c r="D20" s="1084">
-        <v>5.2833125935820373e-15</v>
+        <v>5.283312593582076e-15</v>
       </c>
       <c r="E20" s="1085">
         <v>9.4744164208461664e-42</v>
@@ -42250,7 +42250,7 @@
         <v>0.0085346654935746068</v>
       </c>
       <c r="C33" s="1146">
-        <v>0.0080048107590857329</v>
+        <v>0.0080048107590857311</v>
       </c>
       <c r="D33" s="1147">
         <v>0.0069832902758716273</v>
@@ -42259,7 +42259,7 @@
         <v>0.0085346654935746068</v>
       </c>
       <c r="F33" s="1149">
-        <v>0.0080048107590857329</v>
+        <v>0.0080048107590857311</v>
       </c>
       <c r="G33" s="1150">
         <v>0.0069832902758716273</v>
@@ -42273,7 +42273,7 @@
         <v>108.05434658053271</v>
       </c>
       <c r="C34" s="1153">
-        <v>116.41788305406428</v>
+        <v>116.41788305406429</v>
       </c>
       <c r="D34" s="1154">
         <v>130.06196540559628</v>
@@ -42282,7 +42282,7 @@
         <v>9.114861838105158</v>
       </c>
       <c r="F34" s="1156">
-        <v>8.5069940100144805</v>
+        <v>8.5069940100144823</v>
       </c>
       <c r="G34" s="1157">
         <v>13.137008215070502</v>
@@ -42305,7 +42305,7 @@
         <v>2.0810732190722881e-10</v>
       </c>
       <c r="F35" s="1163">
-        <v>1.0121742889898029e-09</v>
+        <v>1.0121742889897992e-09</v>
       </c>
       <c r="G35" s="1164">
         <v>1.9459213231221925e-14</v>
@@ -42501,22 +42501,22 @@
         <v>1</v>
       </c>
       <c r="B48" s="1222">
-        <v>0.013777392023731653</v>
+        <v>0.013777392023731651</v>
       </c>
       <c r="C48" s="1223">
         <v>0.016821802738893384</v>
       </c>
       <c r="D48" s="1224">
-        <v>0.012713052969122864</v>
+        <v>0.012713052969122863</v>
       </c>
       <c r="E48" s="1225">
-        <v>0.013777392023731653</v>
+        <v>0.013777392023731651</v>
       </c>
       <c r="F48" s="1226">
         <v>0.016821802738893384</v>
       </c>
       <c r="G48" s="1227">
-        <v>0.012713052969122864</v>
+        <v>0.012713052969122863</v>
       </c>
     </row>
     <row r="49">
@@ -42524,16 +42524,16 @@
         <v>2</v>
       </c>
       <c r="B49" s="1229">
-        <v>44.993211102145942</v>
+        <v>44.993211102145949</v>
       </c>
       <c r="C49" s="1230">
         <v>32.313493382356818</v>
       </c>
       <c r="D49" s="1231">
-        <v>45.001350893657055</v>
+        <v>45.001350893657062</v>
       </c>
       <c r="E49" s="1232">
-        <v>27.589466249089547</v>
+        <v>27.589466249089551</v>
       </c>
       <c r="F49" s="1233">
         <v>27.133167330642642</v>
@@ -42818,10 +42818,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="1317">
-        <v>0.0080702480427438158</v>
+        <v>0.0080702480427438175</v>
       </c>
       <c r="C4" s="1318">
-        <v>0.0078300995970379435</v>
+        <v>0.0078300995970379417</v>
       </c>
       <c r="D4" s="1319">
         <v>0.0083518636013061812</v>
@@ -42839,19 +42839,19 @@
         <v>0.011429430684266832</v>
       </c>
       <c r="I4" s="1324">
-        <v>0.027152693997553035</v>
+        <v>0.027152693997553039</v>
       </c>
       <c r="J4" s="1325">
         <v>0.015008460328793629</v>
       </c>
       <c r="K4" s="1326">
-        <v>0.013116358677456795</v>
+        <v>0.013116358677456797</v>
       </c>
       <c r="L4" s="1327">
         <v>0.010317445603009743</v>
       </c>
       <c r="M4" s="1328">
-        <v>0.0084536045565464721</v>
+        <v>0.0084536045565464738</v>
       </c>
     </row>
     <row r="5">
@@ -42859,10 +42859,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="1330">
-        <v>9.0217794533450881</v>
+        <v>9.0217794533450864</v>
       </c>
       <c r="C5" s="1331">
-        <v>9.528304264953082</v>
+        <v>9.5283042649530838</v>
       </c>
       <c r="D5" s="1332">
         <v>12.488813687168403</v>
@@ -42880,19 +42880,19 @@
         <v>66.635245489795935</v>
       </c>
       <c r="I5" s="1337">
-        <v>22.753878224168758</v>
+        <v>22.753878224168755</v>
       </c>
       <c r="J5" s="1338">
         <v>19.99104372495156</v>
       </c>
       <c r="K5" s="1339">
-        <v>11.414360715806318</v>
+        <v>11.414360715806316</v>
       </c>
       <c r="L5" s="1340">
         <v>12.996648322410397</v>
       </c>
       <c r="M5" s="1341">
-        <v>10.118244836847314</v>
+        <v>10.118244836847312</v>
       </c>
     </row>
     <row r="6">
@@ -42900,10 +42900,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1343">
-        <v>2.6431994009041572e-10</v>
+        <v>2.6431994009041758e-10</v>
       </c>
       <c r="C6" s="1344">
-        <v>7.2947438294771729e-11</v>
+        <v>7.2947438294771471e-11</v>
       </c>
       <c r="D6" s="1345">
         <v>7.6011153895367929e-14</v>
@@ -42933,7 +42933,7 @@
         <v>2.6033446712779681e-14</v>
       </c>
       <c r="M6" s="1354">
-        <v>1.6991290261878017e-11</v>
+        <v>1.6991290261878143e-11</v>
       </c>
     </row>
     <row r="7">
@@ -43273,7 +43273,7 @@
         <v>0.0092119916893464732</v>
       </c>
       <c r="C18" s="1461">
-        <v>0.011581727950621902</v>
+        <v>0.011581727950621901</v>
       </c>
       <c r="D18" s="1462">
         <v>0.018159551134710596</v>
@@ -43282,22 +43282,22 @@
         <v>0.024040833720149341</v>
       </c>
       <c r="F18" s="1464">
-        <v>0.017218898799100112</v>
+        <v>0.017218898799100109</v>
       </c>
       <c r="G18" s="1465">
-        <v>0.011230361690972517</v>
+        <v>0.011230361690972515</v>
       </c>
       <c r="H18" s="1466">
         <v>0.01641898756837706</v>
       </c>
       <c r="I18" s="1467">
-        <v>0.023635564833049388</v>
+        <v>0.023635564833049384</v>
       </c>
       <c r="J18" s="1468">
-        <v>0.012881239728280801</v>
+        <v>0.012881239728280803</v>
       </c>
       <c r="K18" s="1469">
-        <v>0.0093854609679935846</v>
+        <v>0.0093854609679935863</v>
       </c>
       <c r="L18" s="1470">
         <v>0.0090189520473105463</v>
@@ -43314,7 +43314,7 @@
         <v>14.450080765027602</v>
       </c>
       <c r="C19" s="1474">
-        <v>13.983468855092681</v>
+        <v>13.983468855092683</v>
       </c>
       <c r="D19" s="1475">
         <v>13.573861039742237</v>
@@ -43323,10 +43323,10 @@
         <v>19.353262177977275</v>
       </c>
       <c r="F19" s="1477">
-        <v>38.051748707230878</v>
+        <v>38.051748707230885</v>
       </c>
       <c r="G19" s="1478">
-        <v>63.984724038397978</v>
+        <v>63.984724038397985</v>
       </c>
       <c r="H19" s="1479">
         <v>40.391257523775231</v>
@@ -43338,7 +43338,7 @@
         <v>16.432949811410339</v>
       </c>
       <c r="K19" s="1482">
-        <v>12.729867469854355</v>
+        <v>12.729867469854353</v>
       </c>
       <c r="L19" s="1483">
         <v>10.014602663986535</v>
@@ -43355,7 +43355,7 @@
         <v>1.4149923632181974e-15</v>
       </c>
       <c r="C20" s="1487">
-        <v>3.5186149888800247e-15</v>
+        <v>3.5186149888800117e-15</v>
       </c>
       <c r="D20" s="1488">
         <v>7.9738086008158924e-15</v>
@@ -43364,7 +43364,7 @@
         <v>3.1570925437711933e-19</v>
       </c>
       <c r="F20" s="1490">
-        <v>3.2281394381013395e-28</v>
+        <v>3.2281394381013162e-28</v>
       </c>
       <c r="G20" s="1491">
         <v>2.4066892996896489e-35</v>
@@ -43379,7 +43379,7 @@
         <v>3.7163375299864795e-17</v>
       </c>
       <c r="K20" s="1495">
-        <v>4.5542238398960586e-14</v>
+        <v>4.5542238398960914e-14</v>
       </c>
       <c r="L20" s="1496">
         <v>2.1875841073764729e-11</v>
@@ -43417,7 +43417,7 @@
         <v>0.42877356157563784</v>
       </c>
       <c r="J21" s="1507">
-        <v>0.18662582301964289</v>
+        <v>0.18662582301964287</v>
       </c>
       <c r="K21" s="1508">
         <v>0.10164047948263372</v>
@@ -43455,10 +43455,10 @@
         <v>0.69577088477229931</v>
       </c>
       <c r="I22" s="1519">
-        <v>0.5247658759613264</v>
+        <v>0.52476587596132629</v>
       </c>
       <c r="J22" s="1520">
-        <v>0.2391018358635405</v>
+        <v>0.23910183586354056</v>
       </c>
       <c r="K22" s="1521">
         <v>0.13995291848001876</v>
@@ -43731,7 +43731,7 @@
         <v>0.066436849619665908</v>
       </c>
       <c r="E33" s="1606">
-        <v>0.055390420593369571</v>
+        <v>0.055390420593369565</v>
       </c>
       <c r="F33" s="1607">
         <v>0.048221032231417396</v>
@@ -43755,7 +43755,7 @@
         <v>0.039194198284560972</v>
       </c>
       <c r="M33" s="1614">
-        <v>0.032065145019217943</v>
+        <v>0.03206514501921795</v>
       </c>
     </row>
     <row r="34">
@@ -43772,7 +43772,7 @@
         <v>10.289561808378402</v>
       </c>
       <c r="E34" s="1619">
-        <v>12.992928199076154</v>
+        <v>12.992928199076156</v>
       </c>
       <c r="F34" s="1620">
         <v>5.0415407658565403</v>
@@ -43796,7 +43796,7 @@
         <v>2.8517787783849951</v>
       </c>
       <c r="M34" s="1627">
-        <v>2.4070833148988644</v>
+        <v>2.407083314898864</v>
       </c>
     </row>
     <row r="35">
@@ -43813,7 +43813,7 @@
         <v>1.122437796800168e-11</v>
       </c>
       <c r="E35" s="1632">
-        <v>2.6235831307867556e-14</v>
+        <v>2.6235831307867373e-14</v>
       </c>
       <c r="F35" s="1633">
         <v>1.7611193861782389e-05</v>
@@ -43837,7 +43837,7 @@
         <v>0.0075537305137625566</v>
       </c>
       <c r="M35" s="1640">
-        <v>0.022023722306827948</v>
+        <v>0.022023722306827961</v>
       </c>
     </row>
     <row r="36">
@@ -44219,7 +44219,7 @@
         <v>0.0090904634851149135</v>
       </c>
       <c r="E4" s="1758">
-        <v>0.017865005999783894</v>
+        <v>0.017865005999783898</v>
       </c>
       <c r="F4" s="1759">
         <v>0.023585394679782296</v>
@@ -44234,16 +44234,16 @@
         <v>0.011462807498754881</v>
       </c>
       <c r="J4" s="1763">
-        <v>0.019223836844277781</v>
+        <v>0.019223836844277784</v>
       </c>
       <c r="K4" s="1764">
         <v>0.046428703144215003</v>
       </c>
       <c r="L4" s="1765">
-        <v>0.0098310411666234655</v>
+        <v>0.0098310411666234637</v>
       </c>
       <c r="M4" s="1766">
-        <v>0.012044609084731987</v>
+        <v>0.012044609084731985</v>
       </c>
       <c r="N4" s="1767">
         <v>0.010560493828618784</v>
@@ -44269,7 +44269,7 @@
         <v>14.464149724205955</v>
       </c>
       <c r="E5" s="1774">
-        <v>7.7787010367961171</v>
+        <v>7.7787010367961154</v>
       </c>
       <c r="F5" s="1775">
         <v>5.3448288992496655</v>
@@ -44284,16 +44284,16 @@
         <v>61.522263174425255</v>
       </c>
       <c r="J5" s="1779">
-        <v>38.729771741332755</v>
+        <v>38.729771741332748</v>
       </c>
       <c r="K5" s="1780">
         <v>14.344317552060994</v>
       </c>
       <c r="L5" s="1781">
-        <v>15.31831918125186</v>
+        <v>15.318319181251864</v>
       </c>
       <c r="M5" s="1782">
-        <v>23.210336320164423</v>
+        <v>23.210336320164426</v>
       </c>
       <c r="N5" s="1783">
         <v>15.462943123944358</v>
@@ -44319,7 +44319,7 @@
         <v>1.377124200213264e-15</v>
       </c>
       <c r="E6" s="1790">
-        <v>7.1638607122543019e-09</v>
+        <v>7.1638607122543275e-09</v>
       </c>
       <c r="F6" s="1791">
         <v>7.2847853650784677e-06</v>
@@ -44334,13 +44334,13 @@
         <v>8.3667785687127701e-35</v>
       </c>
       <c r="J6" s="1795">
-        <v>1.8559465188346836e-28</v>
+        <v>1.8559465188346968e-28</v>
       </c>
       <c r="K6" s="1796">
         <v>1.736165515590065e-15</v>
       </c>
       <c r="L6" s="1797">
-        <v>2.7499064679742232e-16</v>
+        <v>2.749906467974204e-16</v>
       </c>
       <c r="M6" s="1798">
         <v>1.3720840577659198e-21</v>
@@ -44419,7 +44419,7 @@
         <v>0.15113347493052023</v>
       </c>
       <c r="E8" s="1822">
-        <v>0.17949437955386982</v>
+        <v>0.17949437955386985</v>
       </c>
       <c r="F8" s="1823">
         <v>0.18239875336087205</v>
@@ -44443,7 +44443,7 @@
         <v>0.17173329247575553</v>
       </c>
       <c r="M8" s="1830">
-        <v>0.30473849309178785</v>
+        <v>0.3047384930917878</v>
       </c>
       <c r="N8" s="1831">
         <v>0.18596205800120591</v>
@@ -44764,19 +44764,19 @@
         <v>0.01145677941826485</v>
       </c>
       <c r="C18" s="1932">
-        <v>0.012451843930471542</v>
+        <v>0.012451843930471541</v>
       </c>
       <c r="D18" s="1933">
-        <v>0.015020240959860116</v>
+        <v>0.015020240959860117</v>
       </c>
       <c r="E18" s="1934">
-        <v>0.023047979887533612</v>
+        <v>0.023047979887533609</v>
       </c>
       <c r="F18" s="1935">
         <v>0.042641261838417335</v>
       </c>
       <c r="G18" s="1936">
-        <v>0.010110425273591201</v>
+        <v>0.010110425273591203</v>
       </c>
       <c r="H18" s="1937">
         <v>0.011512725861217193</v>
@@ -44785,13 +44785,13 @@
         <v>0.017670181350192202</v>
       </c>
       <c r="J18" s="1939">
-        <v>0.023728349880414036</v>
+        <v>0.02372834988041404</v>
       </c>
       <c r="K18" s="1940">
         <v>0.040277775017226083</v>
       </c>
       <c r="L18" s="1941">
-        <v>0.0068507755539754895</v>
+        <v>0.0068507755539754904</v>
       </c>
       <c r="M18" s="1942">
         <v>0.009965456506042308</v>
@@ -44814,19 +44814,19 @@
         <v>21.626275107929654</v>
       </c>
       <c r="C19" s="1948">
-        <v>20.412515103815227</v>
+        <v>20.412515103815231</v>
       </c>
       <c r="D19" s="1949">
-        <v>16.356664267469863</v>
+        <v>16.35666426746986</v>
       </c>
       <c r="E19" s="1950">
-        <v>11.436207953512241</v>
+        <v>11.436207953512243</v>
       </c>
       <c r="F19" s="1951">
         <v>8.1814969815686212</v>
       </c>
       <c r="G19" s="1952">
-        <v>63.338370719753989</v>
+        <v>63.338370719753975</v>
       </c>
       <c r="H19" s="1953">
         <v>47.535164410653209</v>
@@ -44835,7 +44835,7 @@
         <v>36.234347389549377</v>
       </c>
       <c r="J19" s="1955">
-        <v>27.518470322993132</v>
+        <v>27.518470322993128</v>
       </c>
       <c r="K19" s="1956">
         <v>13.031748952231426</v>
@@ -44864,19 +44864,19 @@
         <v>1.1550019955510427e-20</v>
       </c>
       <c r="C20" s="1964">
-        <v>6.4956016034517058e-20</v>
+        <v>6.4956016034516601e-20</v>
       </c>
       <c r="D20" s="1965">
-        <v>4.2471920588578128e-17</v>
+        <v>4.2471920588578436e-17</v>
       </c>
       <c r="E20" s="1966">
-        <v>7.7075501700196541e-13</v>
+        <v>7.7075501700196268e-13</v>
       </c>
       <c r="F20" s="1967">
         <v>2.407514845012103e-09</v>
       </c>
       <c r="G20" s="1968">
-        <v>3.3223725914222769e-35</v>
+        <v>3.322372591422324e-35</v>
       </c>
       <c r="H20" s="1969">
         <v>2.9447534950720328e-31</v>
@@ -44885,7 +44885,7 @@
         <v>1.4931601880556255e-27</v>
       </c>
       <c r="J20" s="1971">
-        <v>7.6075611601043949e-24</v>
+        <v>7.6075611601044493e-24</v>
       </c>
       <c r="K20" s="1972">
         <v>2.4200921385600198e-14</v>
@@ -45345,10 +45345,10 @@
         <v>0.025281484618554284</v>
       </c>
       <c r="M33" s="2118">
-        <v>0.031128685214211322</v>
+        <v>0.031128685214211319</v>
       </c>
       <c r="N33" s="2119">
-        <v>0.04741230031208124</v>
+        <v>0.047412300312081247</v>
       </c>
       <c r="O33" s="2120">
         <v>0.031514112120697248</v>
@@ -45395,10 +45395,10 @@
         <v>5.0564965565755688</v>
       </c>
       <c r="M34" s="2134">
-        <v>6.8375687688638394</v>
+        <v>6.8375687688638402</v>
       </c>
       <c r="N34" s="2135">
-        <v>3.7931072431733792</v>
+        <v>3.7931072431733788</v>
       </c>
       <c r="O34" s="2136">
         <v>1.4857775153641393</v>
@@ -45445,7 +45445,7 @@
         <v>1.6861697389626221e-05</v>
       </c>
       <c r="M35" s="2150">
-        <v>9.840608206425459e-08</v>
+        <v>9.8406082064253862e-08</v>
       </c>
       <c r="N35" s="2151">
         <v>0.00062396761795732551</v>
@@ -45548,7 +45548,7 @@
         <v>0.28304473048327561</v>
       </c>
       <c r="N37" s="2183">
-        <v>0.29678162676218794</v>
+        <v>0.29678162676218789</v>
       </c>
       <c r="O37" s="2184">
         <v>0.17148671759974971</v>
@@ -45824,16 +45824,16 @@
         <v>0.011735484071055907</v>
       </c>
       <c r="D4" s="2267">
-        <v>0.011991991397408999</v>
+        <v>0.011991991397409</v>
       </c>
       <c r="E4" s="2268">
-        <v>0.022634769987617431</v>
+        <v>0.022634769987617438</v>
       </c>
       <c r="F4" s="2269">
-        <v>0.013027547662324114</v>
+        <v>0.013027547662324116</v>
       </c>
       <c r="G4" s="2270">
-        <v>0.013883701036606936</v>
+        <v>0.013883701036606938</v>
       </c>
       <c r="H4" s="2271">
         <v>0.018395630749295958</v>
@@ -45856,16 +45856,16 @@
         <v>11.451661128346609</v>
       </c>
       <c r="D5" s="2277">
-        <v>12.922568699731771</v>
+        <v>12.922568699731769</v>
       </c>
       <c r="E5" s="2278">
-        <v>30.636139515956671</v>
+        <v>30.636139515956664</v>
       </c>
       <c r="F5" s="2279">
-        <v>55.355595681408566</v>
+        <v>55.355595681408559</v>
       </c>
       <c r="G5" s="2280">
-        <v>49.33114378597962</v>
+        <v>49.331143785979613</v>
       </c>
       <c r="H5" s="2281">
         <v>10.508791007504925</v>
@@ -45888,13 +45888,13 @@
         <v>7.4426592578533356e-13</v>
       </c>
       <c r="D6" s="2287">
-        <v>3.0382864594280305e-14</v>
+        <v>3.0382864594280412e-14</v>
       </c>
       <c r="E6" s="2288">
-        <v>2.7718283476290888e-25</v>
+        <v>2.7718283476291085e-25</v>
       </c>
       <c r="F6" s="2289">
-        <v>2.3830693051999893e-33</v>
+        <v>2.3830693052000231e-33</v>
       </c>
       <c r="G6" s="2290">
         <v>9.1282423494280955e-32</v>
@@ -46171,28 +46171,28 @@
         <v>1</v>
       </c>
       <c r="B18" s="2375">
-        <v>0.016003472647060459</v>
+        <v>0.016003472647060455</v>
       </c>
       <c r="C18" s="2376">
         <v>0.013516808936688801</v>
       </c>
       <c r="D18" s="2377">
-        <v>0.01184055771284773</v>
+        <v>0.011840557712847729</v>
       </c>
       <c r="E18" s="2378">
-        <v>0.020040143962136846</v>
+        <v>0.020040143962136849</v>
       </c>
       <c r="F18" s="2379">
-        <v>0.011690838600026801</v>
+        <v>0.011690838600026803</v>
       </c>
       <c r="G18" s="2380">
-        <v>0.011347518954130626</v>
+        <v>0.011347518954130624</v>
       </c>
       <c r="H18" s="2381">
         <v>0.014325011112801525</v>
       </c>
       <c r="I18" s="2382">
-        <v>0.0099000461537932568</v>
+        <v>0.0099000461537932551</v>
       </c>
       <c r="J18" s="2383">
         <v>0.01061429571504143</v>
@@ -46203,28 +46203,28 @@
         <v>2</v>
       </c>
       <c r="B19" s="2385">
-        <v>15.910385670740535</v>
+        <v>15.910385670740538</v>
       </c>
       <c r="C19" s="2386">
         <v>17.651351369937956</v>
       </c>
       <c r="D19" s="2387">
-        <v>21.881024820031641</v>
+        <v>21.881024820031644</v>
       </c>
       <c r="E19" s="2388">
-        <v>30.275799620990661</v>
+        <v>30.275799620990654</v>
       </c>
       <c r="F19" s="2389">
-        <v>56.128642136610218</v>
+        <v>56.128642136610203</v>
       </c>
       <c r="G19" s="2390">
-        <v>55.301812567560354</v>
+        <v>55.301812567560361</v>
       </c>
       <c r="H19" s="2391">
         <v>9.6786797614947968</v>
       </c>
       <c r="I19" s="2392">
-        <v>10.628148431419158</v>
+        <v>10.628148431419159</v>
       </c>
       <c r="J19" s="2393">
         <v>10.681641018661677</v>
@@ -46235,28 +46235,28 @@
         <v>3</v>
       </c>
       <c r="B20" s="2395">
-        <v>9.3687291577508246e-17</v>
+        <v>9.3687291577507556e-17</v>
       </c>
       <c r="C20" s="2396">
         <v>4.6994979146745178e-18</v>
       </c>
       <c r="D20" s="2397">
-        <v>8.1253030763936646e-21</v>
+        <v>8.1253030763936074e-21</v>
       </c>
       <c r="E20" s="2398">
-        <v>3.9982770874893542e-25</v>
+        <v>3.9982770874893822e-25</v>
       </c>
       <c r="F20" s="2399">
-        <v>1.5357040748049818e-33</v>
+        <v>1.5357040748050035e-33</v>
       </c>
       <c r="G20" s="2400">
-        <v>2.4575945296047457e-33</v>
+        <v>2.4575945296047105e-33</v>
       </c>
       <c r="H20" s="2401">
         <v>5.0099616066019603e-11</v>
       </c>
       <c r="I20" s="2402">
-        <v>5.0018601451821834e-12</v>
+        <v>5.0018601451821664e-12</v>
       </c>
       <c r="J20" s="2403">
         <v>4.408160912663307e-12</v>
@@ -46299,7 +46299,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="2415">
-        <v>0.28856667289899146</v>
+        <v>0.28856667289899152</v>
       </c>
       <c r="C22" s="2416">
         <v>0.26720159893000422</v>
@@ -46539,7 +46539,7 @@
         <v>0.054828014114901714</v>
       </c>
       <c r="G33" s="2490">
-        <v>0.039015829294572819</v>
+        <v>0.039015829294572812</v>
       </c>
       <c r="H33" s="2491">
         <v>0.043707293948491696</v>
@@ -46571,7 +46571,7 @@
         <v>4.8095207115304568</v>
       </c>
       <c r="G34" s="2500">
-        <v>5.44343364678351</v>
+        <v>5.4434336467835109</v>
       </c>
       <c r="H34" s="2501">
         <v>4.3749632140779218</v>
@@ -46603,7 +46603,7 @@
         <v>3.4541456779982952e-05</v>
       </c>
       <c r="G35" s="2510">
-        <v>5.4666728846366122e-06</v>
+        <v>5.466672884636591e-06</v>
       </c>
       <c r="H35" s="2511">
         <v>0.00012085137527106048</v>
@@ -46635,7 +46635,7 @@
         <v>0.16769630576620956</v>
       </c>
       <c r="G36" s="2520">
-        <v>0.14359574313572523</v>
+        <v>0.14359574313572526</v>
       </c>
       <c r="H36" s="2521">
         <v>0.11734844088442165</v>
@@ -46667,7 +46667,7 @@
         <v>0.38896979095312678</v>
       </c>
       <c r="G37" s="2530">
-        <v>0.30247583101016323</v>
+        <v>0.30247583101016318</v>
       </c>
       <c r="H37" s="2531">
         <v>0.29599347461305053</v>

</xml_diff>